<commit_message>
fix fast analysis limit handling
</commit_message>
<xml_diff>
--- a/workspaces/fast_gradient/test_scheds.xlsx
+++ b/workspaces/fast_gradient/test_scheds.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,10 +441,15 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>gdpa_fast</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>hopa</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>pd</t>
         </is>
@@ -463,6 +468,9 @@
       <c r="D2" t="n">
         <v>50</v>
       </c>
+      <c r="E2" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -477,6 +485,9 @@
       <c r="D3" t="n">
         <v>50</v>
       </c>
+      <c r="E3" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -491,6 +502,9 @@
       <c r="D4" t="n">
         <v>50</v>
       </c>
+      <c r="E4" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -505,6 +519,9 @@
       <c r="D5" t="n">
         <v>50</v>
       </c>
+      <c r="E5" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -517,6 +534,9 @@
         <v>50</v>
       </c>
       <c r="D6" t="n">
+        <v>50</v>
+      </c>
+      <c r="E6" t="n">
         <v>49</v>
       </c>
     </row>
@@ -531,6 +551,9 @@
         <v>50</v>
       </c>
       <c r="D7" t="n">
+        <v>50</v>
+      </c>
+      <c r="E7" t="n">
         <v>44</v>
       </c>
     </row>
@@ -545,6 +568,9 @@
         <v>50</v>
       </c>
       <c r="D8" t="n">
+        <v>50</v>
+      </c>
+      <c r="E8" t="n">
         <v>42</v>
       </c>
     </row>
@@ -559,6 +585,9 @@
         <v>50</v>
       </c>
       <c r="D9" t="n">
+        <v>50</v>
+      </c>
+      <c r="E9" t="n">
         <v>41</v>
       </c>
     </row>
@@ -573,6 +602,9 @@
         <v>50</v>
       </c>
       <c r="D10" t="n">
+        <v>50</v>
+      </c>
+      <c r="E10" t="n">
         <v>39</v>
       </c>
     </row>
@@ -587,6 +619,9 @@
         <v>50</v>
       </c>
       <c r="D11" t="n">
+        <v>50</v>
+      </c>
+      <c r="E11" t="n">
         <v>32</v>
       </c>
     </row>
@@ -601,6 +636,9 @@
         <v>49</v>
       </c>
       <c r="D12" t="n">
+        <v>49</v>
+      </c>
+      <c r="E12" t="n">
         <v>25</v>
       </c>
     </row>
@@ -615,6 +653,9 @@
         <v>48</v>
       </c>
       <c r="D13" t="n">
+        <v>48</v>
+      </c>
+      <c r="E13" t="n">
         <v>24</v>
       </c>
     </row>
@@ -626,9 +667,12 @@
         <v>48</v>
       </c>
       <c r="C14" t="n">
+        <v>48</v>
+      </c>
+      <c r="D14" t="n">
         <v>45</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>23</v>
       </c>
     </row>
@@ -640,9 +684,12 @@
         <v>45</v>
       </c>
       <c r="C15" t="n">
+        <v>45</v>
+      </c>
+      <c r="D15" t="n">
         <v>41</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>21</v>
       </c>
     </row>
@@ -654,9 +701,12 @@
         <v>42</v>
       </c>
       <c r="C16" t="n">
+        <v>42</v>
+      </c>
+      <c r="D16" t="n">
         <v>36</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>18</v>
       </c>
     </row>
@@ -668,9 +718,12 @@
         <v>36</v>
       </c>
       <c r="C17" t="n">
+        <v>36</v>
+      </c>
+      <c r="D17" t="n">
         <v>30</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>16</v>
       </c>
     </row>
@@ -682,9 +735,12 @@
         <v>30</v>
       </c>
       <c r="C18" t="n">
+        <v>30</v>
+      </c>
+      <c r="D18" t="n">
         <v>29</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
         <v>11</v>
       </c>
     </row>
@@ -696,9 +752,12 @@
         <v>26</v>
       </c>
       <c r="C19" t="n">
+        <v>26</v>
+      </c>
+      <c r="D19" t="n">
         <v>23</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>6</v>
       </c>
     </row>
@@ -707,12 +766,15 @@
         <v>0.8789473684210527</v>
       </c>
       <c r="B20" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" t="n">
+        <v>19</v>
+      </c>
+      <c r="D20" t="n">
         <v>14</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>6</v>
       </c>
     </row>
@@ -724,9 +786,12 @@
         <v>14</v>
       </c>
       <c r="C21" t="n">
+        <v>14</v>
+      </c>
+      <c r="D21" t="n">
         <v>11</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>5</v>
       </c>
     </row>

</xml_diff>